<commit_message>
Small changes to the spreadsheet.  Mainly just moving figures around.
</commit_message>
<xml_diff>
--- a/doc/Estimators.xlsx
+++ b/doc/Estimators.xlsx
@@ -487,7 +487,8 @@
         <c:axId val="265838856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="3"/>
+          <c:max val="5.5"/>
+          <c:min val="3.25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -523,6 +524,7 @@
         <c:axId val="265841208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.70000000000000007"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -596,6 +598,84 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>keff!$I$2:$I$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>3.1844300000000003E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.0199300000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.9254299999999999E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.8660300000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.9099699999999999E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.79786E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.7923500000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.79739E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.8067599999999999E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>keff!$I$2:$I$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>3.1844300000000003E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.0199300000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.9254299999999999E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.8660300000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.9099699999999999E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.79786E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.7923500000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.79739E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.8067599999999999E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>keff!$A$2:$A$10</c:f>
@@ -684,6 +764,84 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>keff!$K$2:$K$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>3.2847700000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.0199300000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.99055E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.91963E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.9239700000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.8243100000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.7940600000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.75723E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.7294899999999998E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>keff!$K$2:$K$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>3.2847700000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.0199300000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.99055E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.91963E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.9239700000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.8243100000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.7940600000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.75723E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.7294899999999998E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>keff!$A$2:$A$10</c:f>
@@ -773,7 +931,8 @@
         <c:axId val="372103496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="3"/>
+          <c:max val="5.5"/>
+          <c:min val="3.25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -809,6 +968,8 @@
         <c:axId val="372107416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.0000000000000004E-2"/>
+          <c:min val="1.0000000000000002E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1213,7 +1374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>